<commit_message>
Reduce ThermalGenerators & Storages in exampleStochastic for speed up
</commit_message>
<xml_diff>
--- a/data/exampleStochastic/Power_Storage.xlsx
+++ b/data/exampleStochastic/Power_Storage.xlsx
@@ -1544,7 +1544,11 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="10" t="n"/>
+      <c r="A9" s="10" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="B9" s="11" t="n">
         <v/>
       </c>
@@ -1944,7 +1948,11 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="10" t="n"/>
+      <c r="A13" s="10" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="B13" s="11" t="n">
         <v/>
       </c>
@@ -2996,7 +3004,11 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="10" t="n"/>
+      <c r="A9" s="10" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="B9" s="11" t="n">
         <v/>
       </c>
@@ -3396,7 +3408,11 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="10" t="n"/>
+      <c r="A13" s="10" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
       <c r="B13" s="11" t="n">
         <v/>
       </c>

</xml_diff>